<commit_message>
17th March 2023 - HDFS Snapshot
</commit_message>
<xml_diff>
--- a/Day Wise Plan - Data Engineering.xlsx
+++ b/Day Wise Plan - Data Engineering.xlsx
@@ -1,24 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gunjan.Arora\Desktop\Gunjan Virmani\TEK Systems\Schedule\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://allegiscloud-my.sharepoint.com/personal/pdharantej_teksystems_com/Documents/Desktop/Intern Training/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C34C240-2F80-442D-95B8-39172C2F94D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{3C34C240-2F80-442D-95B8-39172C2F94D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17F2BAA8-C123-4D85-B3BB-B2EFF5F4238F}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{DAC0EF18-2D52-4856-8269-C5C7F3F64F9E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{DAC0EF18-2D52-4856-8269-C5C7F3F64F9E}"/>
   </bookViews>
   <sheets>
     <sheet name="Java" sheetId="6" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -27,7 +38,22 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="57">
   <si>
-    <t>Monday</t>
+    <t>Session</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>Assignments / Case Study</t>
+  </si>
+  <si>
+    <t>Assessment</t>
   </si>
   <si>
     <t>Tuesday</t>
@@ -36,44 +62,17 @@
     <t>Wednesday</t>
   </si>
   <si>
+    <t>Orientation</t>
+  </si>
+  <si>
     <t>Thursday</t>
-  </si>
-  <si>
-    <t>Friday</t>
-  </si>
-  <si>
-    <t>Saturday</t>
-  </si>
-  <si>
-    <t>Sunday</t>
-  </si>
-  <si>
-    <t>Day</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Session</t>
-  </si>
-  <si>
-    <t>Topic</t>
-  </si>
-  <si>
-    <t>Assignments / Case Study</t>
-  </si>
-  <si>
-    <t>Assessment</t>
-  </si>
-  <si>
-    <t>OOPS</t>
-  </si>
-  <si>
-    <t>Orientation</t>
   </si>
   <si>
     <t>Python Programming fundamentals, Concepts in Python Objects and Data Structure,Strings, Lists, 
 Tuple, Dictionary</t>
+  </si>
+  <si>
+    <t>Friday</t>
   </si>
   <si>
     <t>Working with Python Shell and Editor IDLE, 
@@ -81,7 +80,22 @@
 Overview of Methods and Modules,</t>
   </si>
   <si>
+    <t xml:space="preserve">Python 1 </t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
     <t>Loops and Conditional Statements, File handling,Math</t>
+  </si>
+  <si>
+    <t>Python 2</t>
   </si>
   <si>
     <t>Object Oriented Programming</t>
@@ -91,30 +105,54 @@
 Python Hyper HTTP-2 Framework,Unit Testing with PyTest</t>
   </si>
   <si>
+    <t>OOPS</t>
+  </si>
+  <si>
+    <t>MCQ - Python 1</t>
+  </si>
+  <si>
     <t>RDDMS - Introduction, Introduction to NoSQL, DDL</t>
   </si>
   <si>
+    <t>File Handling</t>
+  </si>
+  <si>
     <t>DML, DQL - Query - Where clause, Order by</t>
   </si>
   <si>
     <t>Joins, subquery</t>
   </si>
   <si>
+    <t>SQL 1</t>
+  </si>
+  <si>
+    <t>Functions - Aggregate functions, String, Date, Regular Expressions</t>
+  </si>
+  <si>
     <t>Group by, Having clause</t>
   </si>
   <si>
-    <t>Functions - Aggregate functions, String, Date, Regular Expressions</t>
+    <t>MCQ - Python 2</t>
   </si>
   <si>
     <t>SDLC , STLC</t>
   </si>
   <si>
+    <t>SQL 2</t>
+  </si>
+  <si>
     <t>Agile, Scrum</t>
   </si>
   <si>
     <t>Data Warehousing - Understanding, DWH process, Data Integration using Talend Open Studio and Pentaho Data integration tools</t>
   </si>
   <si>
+    <t>Case study - Agile, Scrum</t>
+  </si>
+  <si>
+    <t>Hackathon - Python</t>
+  </si>
+  <si>
     <t>Big Data - tools</t>
   </si>
   <si>
@@ -124,82 +162,55 @@
     <t>Introduction to Big Data; Big Data Pipeline, Examples of Big Data, 4V's of Big Data</t>
   </si>
   <si>
+    <t>Big Data - 1</t>
+  </si>
+  <si>
     <t>Challenges of Traditional Systems (RDBMS and DWH), Features of Big Data, Distributed Systems</t>
   </si>
   <si>
+    <t xml:space="preserve">MCQ - SQL </t>
+  </si>
+  <si>
     <t>Hadoop Installation; HDFS Architecture, Hadoop Core Components - HDFS, YARN, Mapreduce</t>
   </si>
   <si>
+    <t>Big Data - 2</t>
+  </si>
+  <si>
+    <t>MapReduce; Map Phase, Partioning, Shuffle and Sort Phase, Python for BigData Analysis with MapReduce, Distributed Processing in MapReduce</t>
+  </si>
+  <si>
+    <t>Holiday Ugadi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MapReduce Jobs, Hadoop MapReduce Job Work Interaction, Setting Up the Environment for MapReduce Development </t>
+  </si>
+  <si>
+    <t>Mapreduce</t>
+  </si>
+  <si>
+    <t>Hive Introduction Origin of Hive Hadoop Ecosystem, Hive Installation, Big Data ETL, Hive Architecture, Hive Characteristics and Features</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Different Hive Tables and its Differences; Hive DDL, DML Commands,  Different Hive Joins; Hive Partitions; </t>
+  </si>
+  <si>
+    <t>Hive Hadoop - 1</t>
+  </si>
+  <si>
+    <t>MCQ - Hadoop, Big Data</t>
+  </si>
+  <si>
     <t>Hive Bucketing, Working with different FileTypes - Avro, Parquet etc</t>
   </si>
   <si>
-    <t>Hive Introduction Origin of Hive Hadoop Ecosystem, Hive Installation, Big Data ETL, Hive Architecture, Hive Characteristics and Features</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Different Hive Tables and its Differences; Hive DDL, DML Commands,  Different Hive Joins; Hive Partitions; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MapReduce Jobs, Hadoop MapReduce Job Work Interaction, Setting Up the Environment for MapReduce Development </t>
-  </si>
-  <si>
-    <t>MapReduce; Map Phase, Partioning, Shuffle and Sort Phase, Python for BigData Analysis with MapReduce, Distributed Processing in MapReduce</t>
+    <t>Hive Hadoop - 2</t>
   </si>
   <si>
     <t>Informatica</t>
   </si>
   <si>
-    <t xml:space="preserve">Python 1 </t>
-  </si>
-  <si>
-    <t>Python 2</t>
-  </si>
-  <si>
-    <t>File Handling</t>
-  </si>
-  <si>
-    <t>SQL 1</t>
-  </si>
-  <si>
-    <t>SQL 2</t>
-  </si>
-  <si>
-    <t>Case study - Agile, Scrum</t>
-  </si>
-  <si>
-    <t>Big Data - 1</t>
-  </si>
-  <si>
-    <t>Big Data - 2</t>
-  </si>
-  <si>
-    <t>Mapreduce</t>
-  </si>
-  <si>
-    <t>Hive Hadoop - 1</t>
-  </si>
-  <si>
-    <t>Hive Hadoop - 2</t>
-  </si>
-  <si>
-    <t>MCQ - Python 1</t>
-  </si>
-  <si>
-    <t>MCQ - Python 2</t>
-  </si>
-  <si>
-    <t>Hackathon - Python</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCQ - SQL </t>
-  </si>
-  <si>
-    <t>MCQ - Hadoop, Big Data</t>
-  </si>
-  <si>
     <t>MCQ - Hive</t>
-  </si>
-  <si>
-    <t>Holiday Ugadi</t>
   </si>
 </sst>
 </file>
@@ -320,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -333,9 +344,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -664,68 +672,68 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18C298D8-24C2-4A3A-853E-5E46664E6D1D}">
   <dimension ref="B1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:XFD33"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.7265625" customWidth="1"/>
-    <col min="3" max="3" width="14.08984375" customWidth="1"/>
-    <col min="4" max="4" width="13.453125" customWidth="1"/>
-    <col min="5" max="5" width="50.6328125" customWidth="1"/>
-    <col min="6" max="6" width="40.90625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
+    <col min="5" max="5" width="50.5703125" customWidth="1"/>
+    <col min="6" max="6" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="3">
         <v>44613</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="3">
         <f t="shared" ref="C3:C10" si="0">C2+1</f>
         <v>44614</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <f>B3+1</f>
         <v>1</v>
@@ -735,15 +743,15 @@
         <v>44615</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <f>B4+1</f>
         <v>2</v>
@@ -753,43 +761,43 @@
         <v>44616</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
       <c r="C6" s="5">
         <f t="shared" si="0"/>
         <v>44617</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="C7" s="5">
         <f t="shared" si="0"/>
         <v>44618</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <f>B5+1</f>
         <v>3</v>
@@ -799,17 +807,17 @@
         <v>44619</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>17</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <f>B8+1</f>
         <v>4</v>
@@ -819,15 +827,15 @@
         <v>44620</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="2:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <f>B9+1</f>
         <v>5</v>
@@ -837,19 +845,19 @@
         <v>44621</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <f>B10+1</f>
         <v>6</v>
@@ -859,17 +867,17 @@
         <v>44622</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <f>B11+1</f>
         <v>7</v>
@@ -879,41 +887,41 @@
         <v>44623</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="4"/>
       <c r="C13" s="5">
         <f t="shared" si="1"/>
         <v>44624</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="4"/>
       <c r="C14" s="5">
         <f t="shared" si="1"/>
         <v>44625</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <f>B12+1</f>
         <v>8</v>
@@ -923,17 +931,17 @@
         <v>44626</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="2:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
         <f>B15+1</f>
         <v>9</v>
@@ -943,15 +951,15 @@
         <v>44627</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="7"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
         <f>B16+1</f>
         <v>10</v>
@@ -961,17 +969,17 @@
         <v>44628</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
         <f>B17+1</f>
         <v>11</v>
@@ -981,17 +989,17 @@
         <v>44629</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="G18" s="7"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
         <f>B18+1</f>
         <v>12</v>
@@ -1001,41 +1009,41 @@
         <v>44630</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="4"/>
       <c r="C20" s="5">
         <f t="shared" si="1"/>
         <v>44631</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="4"/>
       <c r="C21" s="5">
         <f t="shared" si="1"/>
         <v>44632</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
         <f>B19+1</f>
         <v>13</v>
@@ -1045,19 +1053,19 @@
         <v>44633</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
         <f>B22+1</f>
         <v>14</v>
@@ -1067,15 +1075,15 @@
         <v>44634</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="7"/>
     </row>
-    <row r="24" spans="2:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
         <f>B23+1</f>
         <v>15</v>
@@ -1085,15 +1093,15 @@
         <v>44635</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="7"/>
     </row>
-    <row r="25" spans="2:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
         <f>B24+1</f>
         <v>16</v>
@@ -1103,17 +1111,17 @@
         <v>44636</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="2:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
         <f>B25+1</f>
         <v>17</v>
@@ -1123,43 +1131,43 @@
         <v>44637</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
       <c r="C27" s="5">
         <f t="shared" si="1"/>
         <v>44638</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="4"/>
       <c r="C28" s="5">
         <f t="shared" si="1"/>
         <v>44639</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="2:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B29" s="2">
         <f>B26+1</f>
         <v>18</v>
@@ -1169,17 +1177,17 @@
         <v>44640</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B30" s="2">
         <f>B29+1</f>
         <v>19</v>
@@ -1189,30 +1197,30 @@
         <v>44641</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>37</v>
+        <v>6</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>45</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="7"/>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B31" s="10"/>
-      <c r="C31" s="11">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="9"/>
+      <c r="C31" s="10">
         <f t="shared" si="1"/>
         <v>44642</v>
       </c>
-      <c r="D31" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="F31" s="13"/>
-      <c r="G31" s="14"/>
-    </row>
-    <row r="32" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="D31" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="F31" s="12"/>
+      <c r="G31" s="13"/>
+    </row>
+    <row r="32" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B32" s="2">
         <v>20</v>
       </c>
@@ -1221,17 +1229,17 @@
         <v>44643</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>36</v>
+        <v>9</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G32" s="7"/>
     </row>
-    <row r="33" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B33" s="2">
         <f>B32+1</f>
         <v>21</v>
@@ -1241,39 +1249,39 @@
         <v>44644</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="4"/>
       <c r="C34" s="5">
         <f t="shared" si="1"/>
         <v>44645</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
-      <c r="G34" s="9"/>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="G34" s="8"/>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" s="4"/>
       <c r="C35" s="5">
         <f t="shared" si="1"/>
         <v>44646</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
     </row>
-    <row r="36" spans="2:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B36" s="2">
         <f>B33+1</f>
         <v>22</v>
@@ -1283,19 +1291,19 @@
         <v>44647</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" ht="29" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B37" s="2">
         <f>B36+1</f>
         <v>23</v>
@@ -1305,15 +1313,15 @@
         <v>44648</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
     </row>
-    <row r="38" spans="2:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B38" s="2">
         <f>B37+1</f>
         <v>24</v>
@@ -1323,17 +1331,17 @@
         <v>44649</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="G38" s="7"/>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="2">
         <f>B38+1</f>
         <v>25</v>
@@ -1343,17 +1351,17 @@
         <v>44650</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B40" s="2">
         <f>B39+1</f>
         <v>26</v>
@@ -1363,33 +1371,33 @@
         <v>44651</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E40" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" s="4"/>
       <c r="C41" s="5">
         <f t="shared" si="1"/>
         <v>44652</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B42" s="4"/>
       <c r="C42" s="5">
         <f t="shared" si="1"/>
         <v>44653</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>

</xml_diff>

<commit_message>
New start and Informatica Start
</commit_message>
<xml_diff>
--- a/Day Wise Plan - Data Engineering.xlsx
+++ b/Day Wise Plan - Data Engineering.xlsx
@@ -5,17 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://allegiscloud-my.sharepoint.com/personal/pdharantej_teksystems_com/Documents/Desktop/Intern Training/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://allegiscloud-my.sharepoint.com/personal/pdharantej_teksystems_com/Documents/Desktop/TEK_Training/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{3C34C240-2F80-442D-95B8-39172C2F94D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17F2BAA8-C123-4D85-B3BB-B2EFF5F4238F}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{4D48D5CB-E89C-4166-BEFD-C1A48D38FEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD389DD8-6DD8-4A9E-B649-FBB55F8F67BC}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{DAC0EF18-2D52-4856-8269-C5C7F3F64F9E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Java" sheetId="6" r:id="rId1"/>
+    <sheet name="Data engineering" sheetId="6" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Data engineering'!$B$1:$G$87</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,17 +39,38 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="86">
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
   <si>
     <t>Session</t>
   </si>
   <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Day</t>
-  </si>
-  <si>
     <t>Topic</t>
   </si>
   <si>
@@ -56,23 +80,14 @@
     <t>Assessment</t>
   </si>
   <si>
-    <t>Tuesday</t>
-  </si>
-  <si>
-    <t>Wednesday</t>
+    <t>OOPS</t>
   </si>
   <si>
     <t>Orientation</t>
-  </si>
-  <si>
-    <t>Thursday</t>
   </si>
   <si>
     <t>Python Programming fundamentals, Concepts in Python Objects and Data Structure,Strings, Lists, 
 Tuple, Dictionary</t>
-  </si>
-  <si>
-    <t>Friday</t>
   </si>
   <si>
     <t>Working with Python Shell and Editor IDLE, 
@@ -80,22 +95,7 @@
 Overview of Methods and Modules,</t>
   </si>
   <si>
-    <t xml:space="preserve">Python 1 </t>
-  </si>
-  <si>
-    <t>Saturday</t>
-  </si>
-  <si>
-    <t>Sunday</t>
-  </si>
-  <si>
-    <t>Monday</t>
-  </si>
-  <si>
     <t>Loops and Conditional Statements, File handling,Math</t>
-  </si>
-  <si>
-    <t>Python 2</t>
   </si>
   <si>
     <t>Object Oriented Programming</t>
@@ -105,112 +105,221 @@
 Python Hyper HTTP-2 Framework,Unit Testing with PyTest</t>
   </si>
   <si>
-    <t>OOPS</t>
+    <t>RDDMS - Introduction, Introduction to NoSQL, DDL</t>
+  </si>
+  <si>
+    <t>DML, DQL - Query - Where clause, Order by</t>
+  </si>
+  <si>
+    <t>Joins, subquery</t>
+  </si>
+  <si>
+    <t>Group by, Having clause</t>
+  </si>
+  <si>
+    <t>Functions - Aggregate functions, String, Date, Regular Expressions</t>
+  </si>
+  <si>
+    <t>SDLC , STLC</t>
+  </si>
+  <si>
+    <t>Agile, Scrum</t>
+  </si>
+  <si>
+    <t>Data Warehousing - Understanding, DWH process, Data Integration using Talend Open Studio and Pentaho Data integration tools</t>
+  </si>
+  <si>
+    <t>Big Data - tools</t>
+  </si>
+  <si>
+    <t>DWH System Design and structure, understanding ETL and Related Tools</t>
+  </si>
+  <si>
+    <t>Introduction to Big Data; Big Data Pipeline, Examples of Big Data, 4V's of Big Data</t>
+  </si>
+  <si>
+    <t>Challenges of Traditional Systems (RDBMS and DWH), Features of Big Data, Distributed Systems</t>
+  </si>
+  <si>
+    <t>Hadoop Installation; HDFS Architecture, Hadoop Core Components - HDFS, YARN, Mapreduce</t>
+  </si>
+  <si>
+    <t>Hive Bucketing, Working with different FileTypes - Avro, Parquet etc</t>
+  </si>
+  <si>
+    <t>Hive Introduction Origin of Hive Hadoop Ecosystem, Hive Installation, Big Data ETL, Hive Architecture, Hive Characteristics and Features</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Different Hive Tables and its Differences; Hive DDL, DML Commands,  Different Hive Joins; Hive Partitions; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MapReduce Jobs, Hadoop MapReduce Job Work Interaction, Setting Up the Environment for MapReduce Development </t>
+  </si>
+  <si>
+    <t>MapReduce; Map Phase, Partioning, Shuffle and Sort Phase, Python for BigData Analysis with MapReduce, Distributed Processing in MapReduce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Python 1 </t>
+  </si>
+  <si>
+    <t>Python 2</t>
+  </si>
+  <si>
+    <t>File Handling</t>
+  </si>
+  <si>
+    <t>SQL 1</t>
+  </si>
+  <si>
+    <t>SQL 2</t>
+  </si>
+  <si>
+    <t>Case study - Agile, Scrum</t>
+  </si>
+  <si>
+    <t>Big Data - 1</t>
+  </si>
+  <si>
+    <t>Big Data - 2</t>
+  </si>
+  <si>
+    <t>Mapreduce</t>
+  </si>
+  <si>
+    <t>Hive Hadoop - 1</t>
+  </si>
+  <si>
+    <t>Hive Hadoop - 2</t>
   </si>
   <si>
     <t>MCQ - Python 1</t>
   </si>
   <si>
-    <t>RDDMS - Introduction, Introduction to NoSQL, DDL</t>
-  </si>
-  <si>
-    <t>File Handling</t>
-  </si>
-  <si>
-    <t>DML, DQL - Query - Where clause, Order by</t>
-  </si>
-  <si>
-    <t>Joins, subquery</t>
-  </si>
-  <si>
-    <t>SQL 1</t>
-  </si>
-  <si>
-    <t>Functions - Aggregate functions, String, Date, Regular Expressions</t>
-  </si>
-  <si>
-    <t>Group by, Having clause</t>
-  </si>
-  <si>
     <t>MCQ - Python 2</t>
   </si>
   <si>
-    <t>SDLC , STLC</t>
-  </si>
-  <si>
-    <t>SQL 2</t>
-  </si>
-  <si>
-    <t>Agile, Scrum</t>
-  </si>
-  <si>
-    <t>Data Warehousing - Understanding, DWH process, Data Integration using Talend Open Studio and Pentaho Data integration tools</t>
-  </si>
-  <si>
-    <t>Case study - Agile, Scrum</t>
-  </si>
-  <si>
     <t>Hackathon - Python</t>
   </si>
   <si>
-    <t>Big Data - tools</t>
-  </si>
-  <si>
-    <t>DWH System Design and structure, understanding ETL and Related Tools</t>
-  </si>
-  <si>
-    <t>Introduction to Big Data; Big Data Pipeline, Examples of Big Data, 4V's of Big Data</t>
-  </si>
-  <si>
-    <t>Big Data - 1</t>
-  </si>
-  <si>
-    <t>Challenges of Traditional Systems (RDBMS and DWH), Features of Big Data, Distributed Systems</t>
-  </si>
-  <si>
     <t xml:space="preserve">MCQ - SQL </t>
   </si>
   <si>
-    <t>Hadoop Installation; HDFS Architecture, Hadoop Core Components - HDFS, YARN, Mapreduce</t>
-  </si>
-  <si>
-    <t>Big Data - 2</t>
-  </si>
-  <si>
-    <t>MapReduce; Map Phase, Partioning, Shuffle and Sort Phase, Python for BigData Analysis with MapReduce, Distributed Processing in MapReduce</t>
+    <t>MCQ - Hadoop, Big Data</t>
+  </si>
+  <si>
+    <t>MCQ - Hive</t>
   </si>
   <si>
     <t>Holiday Ugadi</t>
   </si>
   <si>
-    <t xml:space="preserve">MapReduce Jobs, Hadoop MapReduce Job Work Interaction, Setting Up the Environment for MapReduce Development </t>
-  </si>
-  <si>
-    <t>Mapreduce</t>
-  </si>
-  <si>
-    <t>Hive Introduction Origin of Hive Hadoop Ecosystem, Hive Installation, Big Data ETL, Hive Architecture, Hive Characteristics and Features</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Different Hive Tables and its Differences; Hive DDL, DML Commands,  Different Hive Joins; Hive Partitions; </t>
-  </si>
-  <si>
-    <t>Hive Hadoop - 1</t>
-  </si>
-  <si>
-    <t>MCQ - Hadoop, Big Data</t>
-  </si>
-  <si>
-    <t>Hive Bucketing, Working with different FileTypes - Avro, Parquet etc</t>
-  </si>
-  <si>
-    <t>Hive Hadoop - 2</t>
-  </si>
-  <si>
-    <t>Informatica</t>
-  </si>
-  <si>
-    <t>MCQ - Hive</t>
+    <t>Holiday - May Day</t>
+  </si>
+  <si>
+    <t>Capstone project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final Presentation </t>
+  </si>
+  <si>
+    <t>GCP</t>
+  </si>
+  <si>
+    <t>AWS</t>
+  </si>
+  <si>
+    <t>MCQ - Informatica</t>
+  </si>
+  <si>
+    <t>Case Study - Informatica</t>
+  </si>
+  <si>
+    <t>Python - 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pyspark </t>
+  </si>
+  <si>
+    <t>SQL - 3</t>
+  </si>
+  <si>
+    <t>Case Study - Tableau</t>
+  </si>
+  <si>
+    <t>MCQ - Tableau</t>
+  </si>
+  <si>
+    <t>Level of Detail Calculations (LOD), Advanced Table Calculations using 
+Scope and Direction, Index to Ratios, Advanced Mapping – (Layering, WMS 
+– working with a Web Map Service, Distance Calculations etc.)</t>
+  </si>
+  <si>
+    <t>Remote API calls to third party 
+programs - Python, R, Bash or similar programming languages, Tableau 
+limitations &amp; Support, Statistical modelling</t>
+  </si>
+  <si>
+    <t>Data Table 
+schema design/Data Model in data sources, Cross Database Joins</t>
+  </si>
+  <si>
+    <t>Order of 
+execution (in which filters, calculated fields etc. are executed), Best 
+Practices for Dashboard design</t>
+  </si>
+  <si>
+    <t>Comparison of Tableau with other 
+visualizations tools, Admin overview</t>
+  </si>
+  <si>
+    <t>Overview of ETL solution using PowerCenter, Architecture, Cloud Data 
+Management with Informatica, Informatica MDM, SOA, ICC, Designer 
+interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Design data transformations, manage sources and targets 
+definitions, Filter, Join, Aggregate, Categorize, Merge, and </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apply 
+Expression logic without SQL, Monitor and Repair PowerCenter Sessions 
+and Workflows, PowerCenter Repository, </t>
+  </si>
+  <si>
+    <t>Troubleshoot mapping 
+problems, Leverage object reusability, Agile Data integration</t>
+  </si>
+  <si>
+    <t>Informatica Transformations –
+Aggregator / Router / Joiner / Rank Overview</t>
+  </si>
+  <si>
+    <t>Python Language Libraries for DE, Basics of Matplotlib</t>
+  </si>
+  <si>
+    <t>Numpy, pandas, dask, pytyping</t>
+  </si>
+  <si>
+    <t>Pyspark, Spark Streaming</t>
+  </si>
+  <si>
+    <t>Working with GraphX, PySparkSQL/DataFrame 
+Modelling</t>
+  </si>
+  <si>
+    <t>Understanding Spark Architecture / SparkConf / SparkContext / SparkFiles 
+/SparkRDD</t>
+  </si>
+  <si>
+    <t>Spark SQL, DATA FRAMES, creating Data Frames, manual 
+inferring of schema, working with CSV files, reading JDBC tables</t>
+  </si>
+  <si>
+    <t>JSON support in Spark SQL, working with XML data, parquet 
+files, Creating HiveContext</t>
+  </si>
+  <si>
+    <t>MCQ - Pyspark</t>
   </si>
 </sst>
 </file>
@@ -241,7 +350,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -266,8 +375,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -290,48 +405,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -347,13 +425,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -670,11 +743,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18C298D8-24C2-4A3A-853E-5E46664E6D1D}">
-  <dimension ref="B1:G42"/>
+  <dimension ref="B1:G87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -688,31 +759,31 @@
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="C2" s="3">
-        <v>44613</v>
+        <v>44978</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -722,13 +793,13 @@
       <c r="B3" s="2"/>
       <c r="C3" s="3">
         <f t="shared" ref="C3:C10" si="0">C2+1</f>
-        <v>44614</v>
+        <v>44979</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="7"/>
@@ -740,13 +811,13 @@
       </c>
       <c r="C4" s="3">
         <f t="shared" si="0"/>
-        <v>44615</v>
+        <v>44980</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -758,16 +829,16 @@
       </c>
       <c r="C5" s="3">
         <f t="shared" si="0"/>
-        <v>44616</v>
+        <v>44981</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="G5" s="2"/>
     </row>
@@ -775,10 +846,10 @@
       <c r="B6" s="4"/>
       <c r="C6" s="5">
         <f t="shared" si="0"/>
-        <v>44617</v>
+        <v>44982</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -788,10 +859,10 @@
       <c r="B7" s="4"/>
       <c r="C7" s="5">
         <f t="shared" si="0"/>
-        <v>44618</v>
+        <v>44983</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -804,16 +875,16 @@
       </c>
       <c r="C8" s="3">
         <f t="shared" si="0"/>
-        <v>44619</v>
+        <v>44984</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>17</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="G8" s="2"/>
     </row>
@@ -824,13 +895,13 @@
       </c>
       <c r="C9" s="3">
         <f t="shared" si="0"/>
-        <v>44620</v>
+        <v>44985</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -842,19 +913,19 @@
       </c>
       <c r="C10" s="3">
         <f t="shared" si="0"/>
-        <v>44621</v>
+        <v>44986</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>22</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
@@ -863,17 +934,17 @@
         <v>6</v>
       </c>
       <c r="C11" s="3">
-        <f t="shared" ref="C11:C42" si="1">C10+1</f>
-        <v>44622</v>
+        <f t="shared" ref="C11:C74" si="1">C10+1</f>
+        <v>44987</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="G11" s="7"/>
     </row>
@@ -884,13 +955,13 @@
       </c>
       <c r="C12" s="3">
         <f t="shared" si="1"/>
-        <v>44623</v>
+        <v>44988</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
@@ -899,10 +970,10 @@
       <c r="B13" s="4"/>
       <c r="C13" s="5">
         <f t="shared" si="1"/>
-        <v>44624</v>
+        <v>44989</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -912,10 +983,10 @@
       <c r="B14" s="4"/>
       <c r="C14" s="5">
         <f t="shared" si="1"/>
-        <v>44625</v>
+        <v>44990</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -928,16 +999,16 @@
       </c>
       <c r="C15" s="3">
         <f t="shared" si="1"/>
-        <v>44626</v>
+        <v>44991</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="G15" s="2"/>
     </row>
@@ -948,13 +1019,13 @@
       </c>
       <c r="C16" s="3">
         <f t="shared" si="1"/>
-        <v>44627</v>
+        <v>44992</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F16" s="2"/>
       <c r="G16" s="7"/>
@@ -966,17 +1037,17 @@
       </c>
       <c r="C17" s="3">
         <f t="shared" si="1"/>
-        <v>44628</v>
+        <v>44993</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F17" s="2"/>
       <c r="G17" s="7" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
@@ -986,16 +1057,16 @@
       </c>
       <c r="C18" s="3">
         <f t="shared" si="1"/>
-        <v>44629</v>
+        <v>44994</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="G18" s="7"/>
     </row>
@@ -1006,13 +1077,13 @@
       </c>
       <c r="C19" s="3">
         <f t="shared" si="1"/>
-        <v>44630</v>
+        <v>44995</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1021,10 +1092,10 @@
       <c r="B20" s="4"/>
       <c r="C20" s="5">
         <f t="shared" si="1"/>
-        <v>44631</v>
+        <v>44996</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -1034,10 +1105,10 @@
       <c r="B21" s="4"/>
       <c r="C21" s="5">
         <f t="shared" si="1"/>
-        <v>44632</v>
+        <v>44997</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
@@ -1050,19 +1121,19 @@
       </c>
       <c r="C22" s="3">
         <f t="shared" si="1"/>
-        <v>44633</v>
+        <v>44998</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
@@ -1072,13 +1143,13 @@
       </c>
       <c r="C23" s="3">
         <f t="shared" si="1"/>
-        <v>44634</v>
+        <v>44999</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="7"/>
@@ -1090,13 +1161,13 @@
       </c>
       <c r="C24" s="3">
         <f t="shared" si="1"/>
-        <v>44635</v>
+        <v>45000</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="7"/>
@@ -1108,16 +1179,16 @@
       </c>
       <c r="C25" s="3">
         <f t="shared" si="1"/>
-        <v>44636</v>
+        <v>45001</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="G25" s="7"/>
     </row>
@@ -1128,27 +1199,27 @@
       </c>
       <c r="C26" s="3">
         <f t="shared" si="1"/>
-        <v>44637</v>
+        <v>45002</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="7" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="4"/>
       <c r="C27" s="5">
         <f t="shared" si="1"/>
-        <v>44638</v>
+        <v>45003</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
@@ -1158,10 +1229,10 @@
       <c r="B28" s="4"/>
       <c r="C28" s="5">
         <f t="shared" si="1"/>
-        <v>44639</v>
+        <v>45004</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
@@ -1174,16 +1245,16 @@
       </c>
       <c r="C29" s="3">
         <f t="shared" si="1"/>
-        <v>44640</v>
+        <v>45005</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G29" s="2"/>
     </row>
@@ -1194,13 +1265,13 @@
       </c>
       <c r="C30" s="3">
         <f t="shared" si="1"/>
-        <v>44641</v>
+        <v>45006</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="7"/>
@@ -1209,16 +1280,16 @@
       <c r="B31" s="9"/>
       <c r="C31" s="10">
         <f t="shared" si="1"/>
-        <v>44642</v>
+        <v>45007</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>46</v>
+        <v>2</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>55</v>
       </c>
       <c r="F31" s="12"/>
-      <c r="G31" s="13"/>
+      <c r="G31" s="12"/>
     </row>
     <row r="32" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B32" s="2">
@@ -1226,16 +1297,16 @@
       </c>
       <c r="C32" s="3">
         <f t="shared" si="1"/>
-        <v>44643</v>
+        <v>45008</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G32" s="7"/>
     </row>
@@ -1246,23 +1317,25 @@
       </c>
       <c r="C33" s="3">
         <f t="shared" si="1"/>
-        <v>44644</v>
+        <v>45009</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>49</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B34" s="4"/>
       <c r="C34" s="5">
         <f t="shared" si="1"/>
-        <v>44645</v>
+        <v>45010</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
@@ -1272,10 +1345,10 @@
       <c r="B35" s="4"/>
       <c r="C35" s="5">
         <f t="shared" si="1"/>
-        <v>44646</v>
+        <v>45011</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
@@ -1288,19 +1361,19 @@
       </c>
       <c r="C36" s="3">
         <f t="shared" si="1"/>
-        <v>44647</v>
+        <v>45012</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G36" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="37" spans="2:7" ht="30" x14ac:dyDescent="0.25">
@@ -1310,13 +1383,13 @@
       </c>
       <c r="C37" s="3">
         <f t="shared" si="1"/>
-        <v>44648</v>
+        <v>45013</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
@@ -1328,63 +1401,65 @@
       </c>
       <c r="C38" s="3">
         <f t="shared" si="1"/>
-        <v>44649</v>
+        <v>45014</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G38" s="7"/>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B39" s="2">
         <f>B38+1</f>
         <v>25</v>
       </c>
       <c r="C39" s="3">
         <f t="shared" si="1"/>
-        <v>44650</v>
+        <v>45015</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>55</v>
+        <v>3</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>73</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B40" s="2">
         <f>B39+1</f>
         <v>26</v>
       </c>
       <c r="C40" s="3">
         <f t="shared" si="1"/>
-        <v>44651</v>
+        <v>45016</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E40" t="s">
-        <v>55</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B41" s="4"/>
       <c r="C41" s="5">
         <f t="shared" si="1"/>
-        <v>44652</v>
+        <v>45017</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
@@ -1394,18 +1469,740 @@
       <c r="B42" s="4"/>
       <c r="C42" s="5">
         <f t="shared" si="1"/>
-        <v>44653</v>
+        <v>45018</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
     </row>
+    <row r="43" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B43" s="2">
+        <v>27</v>
+      </c>
+      <c r="C43" s="11">
+        <f t="shared" si="1"/>
+        <v>45019</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+    </row>
+    <row r="44" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B44" s="2">
+        <v>28</v>
+      </c>
+      <c r="C44" s="11">
+        <f t="shared" si="1"/>
+        <v>45020</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F44" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="G44" s="2"/>
+    </row>
+    <row r="45" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B45" s="2">
+        <v>29</v>
+      </c>
+      <c r="C45" s="11">
+        <f t="shared" si="1"/>
+        <v>45021</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46" s="2">
+        <v>30</v>
+      </c>
+      <c r="C46" s="11">
+        <f t="shared" si="1"/>
+        <v>45022</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F46" s="2"/>
+      <c r="G46" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47" s="2">
+        <v>31</v>
+      </c>
+      <c r="C47" s="11">
+        <f t="shared" si="1"/>
+        <v>45023</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B48" s="4"/>
+      <c r="C48" s="5">
+        <f t="shared" si="1"/>
+        <v>45024</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B49" s="4"/>
+      <c r="C49" s="5">
+        <f t="shared" si="1"/>
+        <v>45025</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B50" s="2">
+        <v>32</v>
+      </c>
+      <c r="C50" s="11">
+        <f t="shared" si="1"/>
+        <v>45026</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G50" s="2"/>
+    </row>
+    <row r="51" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B51" s="2">
+        <v>33</v>
+      </c>
+      <c r="C51" s="11">
+        <f t="shared" si="1"/>
+        <v>45027</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
+    </row>
+    <row r="52" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B52" s="2">
+        <v>34</v>
+      </c>
+      <c r="C52" s="11">
+        <f t="shared" si="1"/>
+        <v>45028</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+    </row>
+    <row r="53" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B53" s="2">
+        <v>35</v>
+      </c>
+      <c r="C53" s="11">
+        <f t="shared" si="1"/>
+        <v>45029</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F53" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G53" s="2"/>
+    </row>
+    <row r="54" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B54" s="2">
+        <v>36</v>
+      </c>
+      <c r="C54" s="11">
+        <f t="shared" si="1"/>
+        <v>45030</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F54" s="2"/>
+      <c r="G54" s="2"/>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B55" s="4"/>
+      <c r="C55" s="5">
+        <f t="shared" si="1"/>
+        <v>45031</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B56" s="4"/>
+      <c r="C56" s="5">
+        <f t="shared" si="1"/>
+        <v>45032</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+    </row>
+    <row r="57" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B57" s="2">
+        <v>37</v>
+      </c>
+      <c r="C57" s="11">
+        <f t="shared" si="1"/>
+        <v>45033</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G57" s="2"/>
+    </row>
+    <row r="58" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B58" s="2">
+        <v>38</v>
+      </c>
+      <c r="C58" s="11">
+        <f t="shared" si="1"/>
+        <v>45034</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F58" s="2"/>
+      <c r="G58" s="2"/>
+    </row>
+    <row r="59" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B59" s="2">
+        <v>39</v>
+      </c>
+      <c r="C59" s="11">
+        <f t="shared" si="1"/>
+        <v>45035</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F59" s="2"/>
+      <c r="G59" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B60" s="2">
+        <v>40</v>
+      </c>
+      <c r="C60" s="11">
+        <f t="shared" si="1"/>
+        <v>45036</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G60" s="2"/>
+    </row>
+    <row r="61" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B61" s="2">
+        <v>41</v>
+      </c>
+      <c r="C61" s="11">
+        <f t="shared" si="1"/>
+        <v>45037</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F61" s="2"/>
+      <c r="G61" s="2"/>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B62" s="4"/>
+      <c r="C62" s="5">
+        <f t="shared" si="1"/>
+        <v>45038</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4"/>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B63" s="4"/>
+      <c r="C63" s="5">
+        <f t="shared" si="1"/>
+        <v>45039</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="4"/>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B64" s="2">
+        <v>42</v>
+      </c>
+      <c r="C64" s="11">
+        <f t="shared" si="1"/>
+        <v>45040</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F64" s="2"/>
+      <c r="G64" s="7"/>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B65" s="2">
+        <v>43</v>
+      </c>
+      <c r="C65" s="11">
+        <f t="shared" si="1"/>
+        <v>45041</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F65" s="2"/>
+      <c r="G65" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B66" s="2">
+        <v>44</v>
+      </c>
+      <c r="C66" s="11">
+        <f t="shared" si="1"/>
+        <v>45042</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F66" s="2"/>
+      <c r="G66" s="2"/>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B67" s="2">
+        <v>45</v>
+      </c>
+      <c r="C67" s="11">
+        <f t="shared" si="1"/>
+        <v>45043</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F67" s="2"/>
+      <c r="G67" s="2"/>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B68" s="2">
+        <v>46</v>
+      </c>
+      <c r="C68" s="11">
+        <f t="shared" si="1"/>
+        <v>45044</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F68" s="2"/>
+      <c r="G68" s="2"/>
+    </row>
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B69" s="4"/>
+      <c r="C69" s="5">
+        <f t="shared" si="1"/>
+        <v>45045</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E69" s="4"/>
+      <c r="F69" s="4"/>
+      <c r="G69" s="4"/>
+    </row>
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B70" s="4"/>
+      <c r="C70" s="5">
+        <f t="shared" si="1"/>
+        <v>45046</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E70" s="4"/>
+      <c r="F70" s="4"/>
+      <c r="G70" s="4"/>
+    </row>
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B71" s="9"/>
+      <c r="C71" s="10">
+        <f t="shared" si="1"/>
+        <v>45047</v>
+      </c>
+      <c r="D71" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E71" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F71" s="12"/>
+      <c r="G71" s="12"/>
+    </row>
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B72" s="2">
+        <v>47</v>
+      </c>
+      <c r="C72" s="11">
+        <f t="shared" si="1"/>
+        <v>45048</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F72" s="2"/>
+      <c r="G72" s="2"/>
+    </row>
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B73" s="2">
+        <v>48</v>
+      </c>
+      <c r="C73" s="11">
+        <f t="shared" si="1"/>
+        <v>45049</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F73" s="2"/>
+      <c r="G73" s="2"/>
+    </row>
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B74" s="2">
+        <v>49</v>
+      </c>
+      <c r="C74" s="11">
+        <f t="shared" si="1"/>
+        <v>45050</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
+    </row>
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B75" s="2">
+        <v>50</v>
+      </c>
+      <c r="C75" s="11">
+        <f t="shared" ref="C75:C77" si="2">C74+1</f>
+        <v>45051</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F75" s="2"/>
+      <c r="G75" s="2"/>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B76" s="4"/>
+      <c r="C76" s="5">
+        <f t="shared" si="2"/>
+        <v>45052</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E76" s="4"/>
+      <c r="F76" s="4"/>
+      <c r="G76" s="4"/>
+    </row>
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B77" s="4"/>
+      <c r="C77" s="5">
+        <f t="shared" si="2"/>
+        <v>45053</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E77" s="4"/>
+      <c r="F77" s="4"/>
+      <c r="G77" s="4"/>
+    </row>
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B78" s="2">
+        <v>51</v>
+      </c>
+      <c r="C78" s="3">
+        <v>45054</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F78" s="2"/>
+      <c r="G78" s="2"/>
+    </row>
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B79" s="2">
+        <v>52</v>
+      </c>
+      <c r="C79" s="3">
+        <v>45055</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F79" s="2"/>
+      <c r="G79" s="2"/>
+    </row>
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B80" s="2">
+        <v>53</v>
+      </c>
+      <c r="C80" s="3">
+        <v>45056</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F80" s="2"/>
+      <c r="G80" s="2"/>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B81" s="2">
+        <v>54</v>
+      </c>
+      <c r="C81" s="3">
+        <v>45057</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F81" s="2"/>
+      <c r="G81" s="2"/>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B82" s="2">
+        <v>55</v>
+      </c>
+      <c r="C82" s="3">
+        <v>45058</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F82" s="2"/>
+      <c r="G82" s="2"/>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B83" s="4"/>
+      <c r="C83" s="5">
+        <v>45059</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E83" s="4"/>
+      <c r="F83" s="4"/>
+      <c r="G83" s="4"/>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B84" s="4"/>
+      <c r="C84" s="5">
+        <v>45060</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E84" s="4"/>
+      <c r="F84" s="4"/>
+      <c r="G84" s="4"/>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B85" s="2">
+        <v>56</v>
+      </c>
+      <c r="C85" s="3">
+        <v>45061</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F85" s="2"/>
+      <c r="G85" s="2"/>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B86" s="2">
+        <v>57</v>
+      </c>
+      <c r="C86" s="3">
+        <v>45062</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F86" s="2"/>
+      <c r="G86" s="2"/>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B87" s="2">
+        <v>58</v>
+      </c>
+      <c r="C87" s="3">
+        <v>45063</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F87" s="2"/>
+      <c r="G87" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="E31:G31"/>
+    <mergeCell ref="E71:G71"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Day Wise Plan - Data Engineering.xlsx
</commit_message>
<xml_diff>
--- a/Day Wise Plan - Data Engineering.xlsx
+++ b/Day Wise Plan - Data Engineering.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://allegiscloud-my.sharepoint.com/personal/pdharantej_teksystems_com/Documents/Desktop/TEK_Training/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dharantej/Desktop/TEK_Training/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{4D48D5CB-E89C-4166-BEFD-C1A48D38FEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD389DD8-6DD8-4A9E-B649-FBB55F8F67BC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E1974D1-A029-0E40-93ED-5C93E9F1CC6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{DAC0EF18-2D52-4856-8269-C5C7F3F64F9E}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17260" xr2:uid="{DAC0EF18-2D52-4856-8269-C5C7F3F64F9E}"/>
   </bookViews>
   <sheets>
     <sheet name="Data engineering" sheetId="6" r:id="rId1"/>
@@ -444,6 +444,60 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BC245A7-8CCC-2426-BB9B-276484FDF391}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="-7" r="-7"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="10674350" y="20300950"/>
+          <a:ext cx="10096500" cy="8077200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -745,19 +799,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18C298D8-24C2-4A3A-853E-5E46664E6D1D}">
   <dimension ref="B1:G87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="J64" sqref="J64"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" customWidth="1"/>
-    <col min="5" max="5" width="50.5703125" customWidth="1"/>
-    <col min="6" max="6" width="40.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="5" max="5" width="50.5" customWidth="1"/>
+    <col min="6" max="6" width="40.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
@@ -777,7 +833,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B2" s="2"/>
       <c r="C2" s="3">
         <v>44978</v>
@@ -789,7 +845,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" s="2"/>
       <c r="C3" s="3">
         <f t="shared" ref="C3:C10" si="0">C2+1</f>
@@ -804,7 +860,7 @@
       <c r="F3" s="2"/>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" ht="48" x14ac:dyDescent="0.2">
       <c r="B4" s="2">
         <f>B3+1</f>
         <v>1</v>
@@ -822,7 +878,7 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" ht="48" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
         <f>B4+1</f>
         <v>2</v>
@@ -842,7 +898,7 @@
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="4"/>
       <c r="C6" s="5">
         <f t="shared" si="0"/>
@@ -855,7 +911,7 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" s="4"/>
       <c r="C7" s="5">
         <f t="shared" si="0"/>
@@ -868,7 +924,7 @@
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="2">
         <f>B5+1</f>
         <v>3</v>
@@ -888,7 +944,7 @@
       </c>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="2">
         <f>B8+1</f>
         <v>4</v>
@@ -906,7 +962,7 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B10" s="2">
         <f>B9+1</f>
         <v>5</v>
@@ -928,7 +984,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" s="2">
         <f>B10+1</f>
         <v>6</v>
@@ -948,7 +1004,7 @@
       </c>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" s="2">
         <f>B11+1</f>
         <v>7</v>
@@ -966,7 +1022,7 @@
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B13" s="4"/>
       <c r="C13" s="5">
         <f t="shared" si="1"/>
@@ -979,7 +1035,7 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14" s="4"/>
       <c r="C14" s="5">
         <f t="shared" si="1"/>
@@ -992,7 +1048,7 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B15" s="2">
         <f>B12+1</f>
         <v>8</v>
@@ -1012,7 +1068,7 @@
       </c>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B16" s="2">
         <f>B15+1</f>
         <v>9</v>
@@ -1030,7 +1086,7 @@
       <c r="F16" s="2"/>
       <c r="G16" s="7"/>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B17" s="2">
         <f>B16+1</f>
         <v>10</v>
@@ -1050,7 +1106,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B18" s="2">
         <f>B17+1</f>
         <v>11</v>
@@ -1070,7 +1126,7 @@
       </c>
       <c r="G18" s="7"/>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B19" s="2">
         <f>B18+1</f>
         <v>12</v>
@@ -1088,7 +1144,7 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20" s="4"/>
       <c r="C20" s="5">
         <f t="shared" si="1"/>
@@ -1101,7 +1157,7 @@
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" s="4"/>
       <c r="C21" s="5">
         <f t="shared" si="1"/>
@@ -1114,7 +1170,7 @@
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" ht="48" x14ac:dyDescent="0.2">
       <c r="B22" s="2">
         <f>B19+1</f>
         <v>13</v>
@@ -1136,7 +1192,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B23" s="2">
         <f>B22+1</f>
         <v>14</v>
@@ -1154,7 +1210,7 @@
       <c r="F23" s="2"/>
       <c r="G23" s="7"/>
     </row>
-    <row r="24" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B24" s="2">
         <f>B23+1</f>
         <v>15</v>
@@ -1172,7 +1228,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="7"/>
     </row>
-    <row r="25" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B25" s="2">
         <f>B24+1</f>
         <v>16</v>
@@ -1192,7 +1248,7 @@
       </c>
       <c r="G25" s="7"/>
     </row>
-    <row r="26" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B26" s="2">
         <f>B25+1</f>
         <v>17</v>
@@ -1212,7 +1268,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B27" s="4"/>
       <c r="C27" s="5">
         <f t="shared" si="1"/>
@@ -1225,7 +1281,7 @@
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B28" s="4"/>
       <c r="C28" s="5">
         <f t="shared" si="1"/>
@@ -1238,7 +1294,7 @@
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
     </row>
-    <row r="29" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B29" s="2">
         <f>B26+1</f>
         <v>18</v>
@@ -1258,7 +1314,7 @@
       </c>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:7" ht="48" x14ac:dyDescent="0.2">
       <c r="B30" s="2">
         <f>B29+1</f>
         <v>19</v>
@@ -1276,7 +1332,7 @@
       <c r="F30" s="2"/>
       <c r="G30" s="7"/>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B31" s="9"/>
       <c r="C31" s="10">
         <f t="shared" si="1"/>
@@ -1291,7 +1347,7 @@
       <c r="F31" s="12"/>
       <c r="G31" s="12"/>
     </row>
-    <row r="32" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B32" s="2">
         <v>20</v>
       </c>
@@ -1310,7 +1366,7 @@
       </c>
       <c r="G32" s="7"/>
     </row>
-    <row r="33" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" ht="48" x14ac:dyDescent="0.2">
       <c r="B33" s="2">
         <f>B32+1</f>
         <v>21</v>
@@ -1328,7 +1384,7 @@
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B34" s="4"/>
       <c r="C34" s="5">
         <f t="shared" si="1"/>
@@ -1341,7 +1397,7 @@
       <c r="F34" s="4"/>
       <c r="G34" s="8"/>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B35" s="4"/>
       <c r="C35" s="5">
         <f t="shared" si="1"/>
@@ -1354,7 +1410,7 @@
       <c r="F35" s="4"/>
       <c r="G35" s="4"/>
     </row>
-    <row r="36" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B36" s="2">
         <f>B33+1</f>
         <v>22</v>
@@ -1376,7 +1432,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B37" s="2">
         <f>B36+1</f>
         <v>23</v>
@@ -1394,7 +1450,7 @@
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
     </row>
-    <row r="38" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B38" s="2">
         <f>B37+1</f>
         <v>24</v>
@@ -1414,7 +1470,7 @@
       </c>
       <c r="G38" s="7"/>
     </row>
-    <row r="39" spans="2:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:7" ht="80" x14ac:dyDescent="0.2">
       <c r="B39" s="2">
         <f>B38+1</f>
         <v>25</v>
@@ -1434,7 +1490,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B40" s="2">
         <f>B39+1</f>
         <v>26</v>
@@ -1452,7 +1508,7 @@
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B41" s="4"/>
       <c r="C41" s="5">
         <f t="shared" si="1"/>
@@ -1465,7 +1521,7 @@
       <c r="F41" s="4"/>
       <c r="G41" s="4"/>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B42" s="4"/>
       <c r="C42" s="5">
         <f t="shared" si="1"/>
@@ -1478,7 +1534,7 @@
       <c r="F42" s="4"/>
       <c r="G42" s="4"/>
     </row>
-    <row r="43" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:7" ht="64" x14ac:dyDescent="0.2">
       <c r="B43" s="2">
         <v>27</v>
       </c>
@@ -1495,7 +1551,7 @@
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
     </row>
-    <row r="44" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B44" s="2">
         <v>28</v>
       </c>
@@ -1514,7 +1570,7 @@
       </c>
       <c r="G44" s="2"/>
     </row>
-    <row r="45" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B45" s="2">
         <v>29</v>
       </c>
@@ -1531,7 +1587,7 @@
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B46" s="2">
         <v>30</v>
       </c>
@@ -1550,7 +1606,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:7" ht="16" x14ac:dyDescent="0.2">
       <c r="B47" s="2">
         <v>31</v>
       </c>
@@ -1567,7 +1623,7 @@
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B48" s="4"/>
       <c r="C48" s="5">
         <f t="shared" si="1"/>
@@ -1580,7 +1636,7 @@
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B49" s="4"/>
       <c r="C49" s="5">
         <f t="shared" si="1"/>
@@ -1593,7 +1649,7 @@
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B50" s="2">
         <v>32</v>
       </c>
@@ -1612,7 +1668,7 @@
       </c>
       <c r="G50" s="2"/>
     </row>
-    <row r="51" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B51" s="2">
         <v>33</v>
       </c>
@@ -1629,7 +1685,7 @@
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
     </row>
-    <row r="52" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:7" ht="48" x14ac:dyDescent="0.2">
       <c r="B52" s="2">
         <v>34</v>
       </c>
@@ -1646,7 +1702,7 @@
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
     </row>
-    <row r="53" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B53" s="2">
         <v>35</v>
       </c>
@@ -1665,7 +1721,7 @@
       </c>
       <c r="G53" s="2"/>
     </row>
-    <row r="54" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B54" s="2">
         <v>36</v>
       </c>
@@ -1682,7 +1738,7 @@
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B55" s="4"/>
       <c r="C55" s="5">
         <f t="shared" si="1"/>
@@ -1695,7 +1751,7 @@
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B56" s="4"/>
       <c r="C56" s="5">
         <f t="shared" si="1"/>
@@ -1708,7 +1764,7 @@
       <c r="F56" s="4"/>
       <c r="G56" s="4"/>
     </row>
-    <row r="57" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:7" ht="80" x14ac:dyDescent="0.2">
       <c r="B57" s="2">
         <v>37</v>
       </c>
@@ -1727,7 +1783,7 @@
       </c>
       <c r="G57" s="2"/>
     </row>
-    <row r="58" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B58" s="2">
         <v>38</v>
       </c>
@@ -1744,7 +1800,7 @@
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
     </row>
-    <row r="59" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:7" ht="64" x14ac:dyDescent="0.2">
       <c r="B59" s="2">
         <v>39</v>
       </c>
@@ -1763,7 +1819,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="60" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:7" ht="32" x14ac:dyDescent="0.2">
       <c r="B60" s="2">
         <v>40</v>
       </c>
@@ -1782,7 +1838,7 @@
       </c>
       <c r="G60" s="2"/>
     </row>
-    <row r="61" spans="2:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:7" ht="64" x14ac:dyDescent="0.2">
       <c r="B61" s="2">
         <v>41</v>
       </c>
@@ -1799,7 +1855,7 @@
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B62" s="4"/>
       <c r="C62" s="5">
         <f t="shared" si="1"/>
@@ -1812,7 +1868,7 @@
       <c r="F62" s="4"/>
       <c r="G62" s="4"/>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B63" s="4"/>
       <c r="C63" s="5">
         <f t="shared" si="1"/>
@@ -1825,7 +1881,7 @@
       <c r="F63" s="4"/>
       <c r="G63" s="4"/>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B64" s="2">
         <v>42</v>
       </c>
@@ -1842,7 +1898,7 @@
       <c r="F64" s="2"/>
       <c r="G64" s="7"/>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B65" s="2">
         <v>43</v>
       </c>
@@ -1861,7 +1917,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B66" s="2">
         <v>44</v>
       </c>
@@ -1878,7 +1934,7 @@
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
     </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B67" s="2">
         <v>45</v>
       </c>
@@ -1895,7 +1951,7 @@
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
     </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B68" s="2">
         <v>46</v>
       </c>
@@ -1912,7 +1968,7 @@
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
     </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B69" s="4"/>
       <c r="C69" s="5">
         <f t="shared" si="1"/>
@@ -1925,7 +1981,7 @@
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B70" s="4"/>
       <c r="C70" s="5">
         <f t="shared" si="1"/>
@@ -1938,7 +1994,7 @@
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B71" s="9"/>
       <c r="C71" s="10">
         <f t="shared" si="1"/>
@@ -1953,7 +2009,7 @@
       <c r="F71" s="12"/>
       <c r="G71" s="12"/>
     </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B72" s="2">
         <v>47</v>
       </c>
@@ -1970,7 +2026,7 @@
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
     </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B73" s="2">
         <v>48</v>
       </c>
@@ -1987,7 +2043,7 @@
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
     </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B74" s="2">
         <v>49</v>
       </c>
@@ -2004,7 +2060,7 @@
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
     </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B75" s="2">
         <v>50</v>
       </c>
@@ -2021,7 +2077,7 @@
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
     </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B76" s="4"/>
       <c r="C76" s="5">
         <f t="shared" si="2"/>
@@ -2034,7 +2090,7 @@
       <c r="F76" s="4"/>
       <c r="G76" s="4"/>
     </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B77" s="4"/>
       <c r="C77" s="5">
         <f t="shared" si="2"/>
@@ -2047,7 +2103,7 @@
       <c r="F77" s="4"/>
       <c r="G77" s="4"/>
     </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B78" s="2">
         <v>51</v>
       </c>
@@ -2063,7 +2119,7 @@
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
     </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B79" s="2">
         <v>52</v>
       </c>
@@ -2079,7 +2135,7 @@
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
     </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B80" s="2">
         <v>53</v>
       </c>
@@ -2095,7 +2151,7 @@
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
     </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B81" s="2">
         <v>54</v>
       </c>
@@ -2111,7 +2167,7 @@
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
     </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B82" s="2">
         <v>55</v>
       </c>
@@ -2127,7 +2183,7 @@
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
     </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B83" s="4"/>
       <c r="C83" s="5">
         <v>45059</v>
@@ -2139,7 +2195,7 @@
       <c r="F83" s="4"/>
       <c r="G83" s="4"/>
     </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B84" s="4"/>
       <c r="C84" s="5">
         <v>45060</v>
@@ -2151,7 +2207,7 @@
       <c r="F84" s="4"/>
       <c r="G84" s="4"/>
     </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B85" s="2">
         <v>56</v>
       </c>
@@ -2167,7 +2223,7 @@
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
     </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B86" s="2">
         <v>57</v>
       </c>
@@ -2183,7 +2239,7 @@
       <c r="F86" s="2"/>
       <c r="G86" s="2"/>
     </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B87" s="2">
         <v>58</v>
       </c>
@@ -2206,5 +2262,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>